<commit_message>
Update notebooks 1,2, 4-13
And delete old fig_NN.html files and notebooks
</commit_message>
<xml_diff>
--- a/ewhr/data/list_of_tables_for_summary.xlsx
+++ b/ewhr/data/list_of_tables_for_summary.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
   <si>
     <t>fig_id</t>
   </si>
@@ -77,9 +78,6 @@
     <t>http://vizhub.healthdata.org/irank/arrow.php</t>
   </si>
   <si>
-    <t xml:space="preserve">Score </t>
-  </si>
-  <si>
     <t>http://reports.weforum.org/global-gender-gap-report-2014/rankings/</t>
   </si>
   <si>
@@ -92,9 +90,6 @@
     <t>Eurostat</t>
   </si>
   <si>
-    <t>http://ec.europa.eu/eurostat/tgm/table.do?tab=table&amp;init=1&amp;plugin=1&amp;language=en&amp;pcode=tsdsc340</t>
-  </si>
-  <si>
     <t>Accessed 16 June 2015</t>
   </si>
   <si>
@@ -122,9 +117,6 @@
     <t>Global Youth Tobacco Survey (GYTS)</t>
   </si>
   <si>
-    <t>http://nccd.cdc.gov/gtssdata/Ancillary/Documentation.aspx?SUID=1&amp;DOCT=1</t>
-  </si>
-  <si>
     <t>Accessed 30 June 2015</t>
   </si>
   <si>
@@ -233,9 +225,6 @@
     <t>Healthy life at birth and number of years spent in ill-health for women (2012)</t>
   </si>
   <si>
-    <t>Female life expectancy at birth (2013) by estimated Gross National Income (GNI) PPP$ per capita (2011)</t>
-  </si>
-  <si>
     <t>Mortality and disease burden (DALYs) in females by sub-region, age group and broad causes (2010)</t>
   </si>
   <si>
@@ -248,27 +237,12 @@
     <t>Gender pay gap (%) in selected Member States (2013)</t>
   </si>
   <si>
-    <t>Probability of dying (per 1000) before 5 years for girls and boys, WHO European Region (2000-2012)</t>
-  </si>
-  <si>
     <t>Pre-primary School Participation for girls (2000-2012)</t>
   </si>
   <si>
-    <t>The Risk of poverty and social exclusion for girls age less than 6 years in the EU (2013)</t>
-  </si>
-  <si>
-    <t>Prevalence of current smoked tobacco use among adolescents girls age 13-15 years in selected countries</t>
-  </si>
-  <si>
-    <t>Adolescents birth rates (2010-2015) by means years of schooling (2002-2012)</t>
-  </si>
-  <si>
     <t>Differences in adolescents in attitudes towards wife beating (2009-2013)</t>
   </si>
   <si>
-    <t>Differences in bad-very bad self-reported health among women aged 18-44 years by highest and lowest equivalised income quintiles in selected EU Member States (2013)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unmet needs for family planning, total, percentage (last year available) </t>
   </si>
   <si>
@@ -291,9 +265,6 @@
   </si>
   <si>
     <t>Percentage</t>
-  </si>
-  <si>
-    <t>Prevalence</t>
   </si>
   <si>
     <t>Number of responses</t>
@@ -385,13 +356,139 @@
   </si>
   <si>
     <t>plot_height</t>
+  </si>
+  <si>
+    <t>Insert standard plot properties code</t>
+  </si>
+  <si>
+    <t>paste plot width constant</t>
+  </si>
+  <si>
+    <t>paste plot height</t>
+  </si>
+  <si>
+    <t>adjust vertical or horizontal orientation</t>
+  </si>
+  <si>
+    <t>insert hovermode property</t>
+  </si>
+  <si>
+    <t>adjust hovermode property</t>
+  </si>
+  <si>
+    <t>check fig_no</t>
+  </si>
+  <si>
+    <t>check fig_id</t>
+  </si>
+  <si>
+    <t>check x_label</t>
+  </si>
+  <si>
+    <t>check y_label</t>
+  </si>
+  <si>
+    <t>adjust width and height</t>
+  </si>
+  <si>
+    <t>check legend (hide or re-position)</t>
+  </si>
+  <si>
+    <t>check source label</t>
+  </si>
+  <si>
+    <t>check source link</t>
+  </si>
+  <si>
+    <t>check date accessed for source</t>
+  </si>
+  <si>
+    <t>check footnotes</t>
+  </si>
+  <si>
+    <t>check caption</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>closest</t>
+  </si>
+  <si>
+    <t>GNI per capita (USD, at PPP)</t>
+  </si>
+  <si>
+    <t>Female Life Expectancy (Years)</t>
+  </si>
+  <si>
+    <t>Female life expectancy at birth (2013) by estimated GNI PPP$ per capita (2011)</t>
+  </si>
+  <si>
+    <t>Score (0=Inequality / 1=Equality)</t>
+  </si>
+  <si>
+    <t>http://bit.ly/tsdsc340</t>
+  </si>
+  <si>
+    <t>The data for the following countries is provisional - Germany, Spain, France, Croatia, Luxembourg, Poland, and Finland.  The data for Romania is estimated.</t>
+  </si>
+  <si>
+    <t>This represents the difference between average gross hourly earnings of male paid employees and female paid employees as a percentage of gross hourly earnings of male paid employees.  The population consists of all paid employees in enterprises with 10 employees or more.</t>
+  </si>
+  <si>
+    <t>Probability of dying before 5 years per 1000 live births</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Rate per 1000, girls and boys, WHO European Region (2000-2012)</t>
+  </si>
+  <si>
+    <t>% of eligible population</t>
+  </si>
+  <si>
+    <t>Risk of poverty and social exclusion for girls age less than 6 years in the EU (2013)</t>
+  </si>
+  <si>
+    <t>http://1.usa.gov/1L02Ezu</t>
+  </si>
+  <si>
+    <t>Current smoked tobacco use, adolescents girls aged 13-15 years, in selected countries</t>
+  </si>
+  <si>
+    <t>Prevalence (%)</t>
+  </si>
+  <si>
+    <t>Mean years of schooling (female, 2002-2012)</t>
+  </si>
+  <si>
+    <t>Births per 1,000 women aged 15-19 (2010/2015)</t>
+  </si>
+  <si>
+    <t>Adolescents birth rates (2010-2015) by mean years of schooling (2002-2012)</t>
+  </si>
+  <si>
+    <t>Quintile 1 is the lowest equivalised income (lowest 20%) and Quintile 5 is the highest equivalised income. Data for the Czech Republic, Croatia, Serbia and UK(5th quintile only) is noted as having low reliability.</t>
+  </si>
+  <si>
+    <t>Percentage reporting bad or very-bad health (%)</t>
+  </si>
+  <si>
+    <t>Self-reported health, women aged 18-44, by high and low income quintiles (2013)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,14 +637,28 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -891,17 +1002,26 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -949,6 +1069,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFD579"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1244,43 +1369,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47" style="4" customWidth="1"/>
     <col min="4" max="4" width="53.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="52.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="85.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="82" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.1640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="13.5" style="3" customWidth="1"/>
+    <col min="6" max="7" width="13" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.6640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="52.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="85.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="82" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -1288,944 +1413,2054 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="b">
+      <c r="H2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K2" s="3">
-        <v>780</v>
+        <v>77</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="L2" s="3">
-        <v>1262</v>
+        <v>960</v>
       </c>
       <c r="M2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="3">
         <v>34</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>63</v>
+      <c r="C3" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="E3" s="3">
         <v>11</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="b">
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="I3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="3">
         <v>780</v>
       </c>
-      <c r="L3" s="3">
-        <v>1262</v>
-      </c>
       <c r="M3" s="3">
+        <v>900</v>
+      </c>
+      <c r="N3" s="3">
         <v>39</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>64</v>
+      <c r="C4" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L4" s="3">
+        <v>780</v>
+      </c>
+      <c r="M4" s="3">
+        <v>900</v>
+      </c>
+      <c r="N4" s="3">
+        <v>41</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K4" s="3">
-        <v>780</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1262</v>
-      </c>
-      <c r="M4" s="3">
-        <v>41</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
+      <c r="C5" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E5" s="3">
         <v>15</v>
       </c>
-      <c r="G5" s="6" t="b">
+      <c r="H5" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="3">
+        <v>960</v>
+      </c>
+      <c r="M5" s="3">
+        <v>780</v>
+      </c>
+      <c r="N5" s="3">
+        <v>44</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="3">
-        <v>780</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1262</v>
-      </c>
-      <c r="M5" s="3">
-        <v>44</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>65</v>
+      <c r="C6" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E6" s="3">
         <v>21</v>
       </c>
-      <c r="G6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>94</v>
+      <c r="H6" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K6" s="3">
+        <v>128</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" s="3">
         <v>780</v>
       </c>
-      <c r="L6" s="3">
-        <v>1262</v>
-      </c>
       <c r="M6" s="3">
+        <v>900</v>
+      </c>
+      <c r="N6" s="3">
         <v>62</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R6" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>53</v>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E7" s="3">
         <v>24</v>
       </c>
-      <c r="G7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>94</v>
+      <c r="F7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" s="3">
+        <v>79</v>
+      </c>
+      <c r="L7" s="3">
         <v>780</v>
       </c>
-      <c r="L7" s="3">
-        <v>1262</v>
-      </c>
       <c r="M7" s="3">
+        <v>900</v>
+      </c>
+      <c r="N7" s="3">
         <v>72</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>54</v>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="E8" s="3">
         <v>32</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L8" s="3">
         <v>780</v>
       </c>
-      <c r="L8" s="3">
-        <v>1262</v>
-      </c>
       <c r="M8" s="3">
+        <v>900</v>
+      </c>
+      <c r="N8" s="3">
         <v>108</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="Q8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3">
         <v>9</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>55</v>
+      <c r="C9" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E9" s="3">
         <v>39</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6" t="b">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="3">
+        <v>84</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" s="3">
         <v>780</v>
       </c>
-      <c r="L9" s="3">
-        <v>1262</v>
-      </c>
       <c r="M9" s="3">
+        <v>900</v>
+      </c>
+      <c r="N9" s="3">
         <v>121</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="O9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>56</v>
+      <c r="C10" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="E10" s="3">
         <v>41</v>
       </c>
-      <c r="G10" s="6" t="b">
+      <c r="H10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I10" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="3">
+        <v>79</v>
+      </c>
+      <c r="L10" s="3">
         <v>780</v>
       </c>
-      <c r="L10" s="3">
-        <v>1262</v>
-      </c>
       <c r="M10" s="3">
+        <v>640</v>
+      </c>
+      <c r="N10" s="3">
         <v>80</v>
       </c>
-      <c r="N10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>29</v>
+      <c r="O10" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>57</v>
+      <c r="C11" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
       <c r="E11" s="3">
         <v>50</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6" t="b">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="3">
+        <v>145</v>
+      </c>
+      <c r="L11" s="3">
         <v>780</v>
       </c>
-      <c r="L11" s="3">
-        <v>1262</v>
-      </c>
       <c r="M11" s="3">
+        <v>640</v>
+      </c>
+      <c r="N11" s="3">
         <v>186</v>
       </c>
-      <c r="N11" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="O11" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>58</v>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>78</v>
+        <v>148</v>
       </c>
       <c r="E12" s="3">
         <v>56</v>
       </c>
-      <c r="G12" s="6" t="b">
+      <c r="H12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K12" s="3">
+      <c r="I12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="L12" s="3">
         <v>780</v>
       </c>
-      <c r="L12" s="3">
-        <v>1262</v>
-      </c>
       <c r="M12" s="3">
+        <v>780</v>
+      </c>
+      <c r="N12" s="3">
         <v>203</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O12" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>59</v>
+      <c r="C13" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E13" s="3">
         <v>57</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="6" t="b">
+      <c r="F13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I13" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="3">
+        <v>79</v>
+      </c>
+      <c r="L13" s="3">
         <v>780</v>
       </c>
-      <c r="L13" s="3">
-        <v>1262</v>
-      </c>
       <c r="M13" s="3">
+        <v>640</v>
+      </c>
+      <c r="N13" s="3">
         <v>121</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="O13" s="3" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>39</v>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="E14" s="3">
         <v>63</v>
       </c>
-      <c r="G14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>94</v>
+      <c r="F14" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K14" s="3">
+        <v>150</v>
+      </c>
+      <c r="L14" s="3">
         <v>780</v>
       </c>
-      <c r="L14" s="3">
-        <v>1262</v>
-      </c>
       <c r="M14" s="3">
+        <v>640</v>
+      </c>
+      <c r="N14" s="3">
         <v>235</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="O14" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>15</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>60</v>
+      <c r="C15" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E15" s="3">
         <v>73</v>
       </c>
-      <c r="G15" s="6" t="b">
+      <c r="H15" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="I15" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L15" s="3">
+        <v>780</v>
+      </c>
+      <c r="M15" s="3">
+        <v>900</v>
+      </c>
+      <c r="N15" s="3">
+        <v>278</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="3">
-        <v>780</v>
-      </c>
-      <c r="L15" s="3">
-        <v>1262</v>
-      </c>
-      <c r="M15" s="3">
-        <v>278</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="P15" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>66</v>
+      <c r="C16" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3">
         <v>78</v>
       </c>
-      <c r="G16" s="6" t="b">
+      <c r="H16" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="I16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="3">
         <v>780</v>
       </c>
-      <c r="L16" s="3">
-        <v>1262</v>
-      </c>
-      <c r="M16" s="8">
+      <c r="M16" s="3">
+        <v>900</v>
+      </c>
+      <c r="N16" s="7">
         <v>39203</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="O16" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3">
         <v>16</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>67</v>
+      <c r="C17" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E17" s="3">
         <v>89</v>
       </c>
-      <c r="G17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>94</v>
+      <c r="H17" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="3">
+        <v>79</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L17" s="3">
         <v>780</v>
       </c>
-      <c r="L17" s="3">
-        <v>1262</v>
-      </c>
       <c r="M17" s="3">
+        <v>900</v>
+      </c>
+      <c r="N17" s="3">
         <v>235</v>
       </c>
-      <c r="N17" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="O17" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3">
         <v>18</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>61</v>
+      <c r="C18" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E18" s="3">
         <v>93</v>
       </c>
-      <c r="G18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>94</v>
+      <c r="H18" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="3">
+        <v>80</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="3">
         <v>780</v>
       </c>
-      <c r="L18" s="3">
-        <v>1262</v>
-      </c>
       <c r="M18" s="3">
+        <v>900</v>
+      </c>
+      <c r="N18" s="3">
         <v>296</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="O18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="R18" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S18" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3">
         <v>97</v>
       </c>
-      <c r="G19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>94</v>
+      <c r="H19" s="4" t="b">
+        <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="3">
+        <v>79</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="3">
         <v>780</v>
       </c>
-      <c r="L19" s="3">
-        <v>1262</v>
-      </c>
       <c r="M19" s="3">
+        <v>900</v>
+      </c>
+      <c r="N19" s="3">
         <v>80</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="O19" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>117</v>
+      <c r="C23" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:S19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="19" width="7.5" style="9" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B1" s="12">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12">
+        <v>10</v>
+      </c>
+      <c r="L1" s="12">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12">
+        <v>14</v>
+      </c>
+      <c r="P1" s="12">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="12">
+        <v>16</v>
+      </c>
+      <c r="R1" s="12">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="11">
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>0</v>
+      </c>
+      <c r="R2" s="11">
+        <v>0</v>
+      </c>
+      <c r="S2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="11">
+        <v>0</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0</v>
+      </c>
+      <c r="N3" s="11">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0</v>
+      </c>
+      <c r="P3" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0</v>
+      </c>
+      <c r="R3" s="11">
+        <v>0</v>
+      </c>
+      <c r="S3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="11">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0</v>
+      </c>
+      <c r="P4" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="11">
+        <v>0</v>
+      </c>
+      <c r="S4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11">
+        <v>0</v>
+      </c>
+      <c r="S5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11">
+        <v>0</v>
+      </c>
+      <c r="S6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>0</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0</v>
+      </c>
+      <c r="S8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>0</v>
+      </c>
+      <c r="R9" s="11">
+        <v>0</v>
+      </c>
+      <c r="S9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="11">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
+        <v>0</v>
+      </c>
+      <c r="S10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>0</v>
+      </c>
+      <c r="R12" s="11">
+        <v>0</v>
+      </c>
+      <c r="S12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0</v>
+      </c>
+      <c r="S13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
+        <v>0</v>
+      </c>
+      <c r="P14" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0</v>
+      </c>
+      <c r="S14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0</v>
+      </c>
+      <c r="M15" s="11">
+        <v>0</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0</v>
+      </c>
+      <c r="O15" s="11">
+        <v>0</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>0</v>
+      </c>
+      <c r="R15" s="11">
+        <v>0</v>
+      </c>
+      <c r="S15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="11">
+        <v>0</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>0</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11">
+        <v>0</v>
+      </c>
+      <c r="P16" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>0</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0</v>
+      </c>
+      <c r="S16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0</v>
+      </c>
+      <c r="P17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
+        <v>0</v>
+      </c>
+      <c r="S17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="11">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0</v>
+      </c>
+      <c r="S18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="23" type="noConversion"/>
+  <conditionalFormatting sqref="B2:S18">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update notebooks 14, 15
Need to check source of data for Notebook 15
</commit_message>
<xml_diff>
--- a/ewhr/data/list_of_tables_for_summary.xlsx
+++ b/ewhr/data/list_of_tables_for_summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="153">
   <si>
     <t>fig_id</t>
   </si>
@@ -147,15 +147,9 @@
     <t>Problems with the original link. I have changed it</t>
   </si>
   <si>
-    <t>http://unstats.un.org/unsd/mdg/SeriesDetail.aspx?srid=764&amp;crid=</t>
-  </si>
-  <si>
     <t>Accessed 26 May 2015</t>
   </si>
   <si>
-    <t>Accessed 16 March 2015</t>
-  </si>
-  <si>
     <t>Will wait to change until you have tried the new version</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>Do European countries maximize the education gain?</t>
   </si>
   <si>
-    <t>Risk of maternal mortality by secondary education (2005-2012)</t>
-  </si>
-  <si>
     <t>Self-perceived health by income in older women</t>
   </si>
   <si>
@@ -244,9 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">Unmet needs for family planning, total, percentage (last year available) </t>
-  </si>
-  <si>
-    <t>Maternal mortality ratio compared to the female population with at least some secondary education (2005-2012)</t>
   </si>
   <si>
     <t>Differences among women aged 65+ in EU countries for self-rated health very good-good by wealth quintiles (2013)</t>
@@ -482,6 +470,21 @@
   </si>
   <si>
     <t>Self-reported health, women aged 18-44, by high and low income quintiles (2013)</t>
+  </si>
+  <si>
+    <t>http://bit.ly/unmet_need_fp</t>
+  </si>
+  <si>
+    <t>Maternal mortality ratio (deaths per 100,000 live births), 2010</t>
+  </si>
+  <si>
+    <t>Risk of maternal mortality by Schooling (2005-2012)</t>
+  </si>
+  <si>
+    <t>Maternal mortality ratio compared to the mean number of years in school, females, 2005-2012</t>
+  </si>
+  <si>
+    <t>Mean Number of Years in School (Females)</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,13 +1402,13 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -1414,16 +1417,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>4</v>
@@ -1432,10 +1435,10 @@
         <v>5</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>6</v>
@@ -1450,10 +1453,10 @@
         <v>9</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1467,7 +1470,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3">
         <v>10</v>
@@ -1476,13 +1479,13 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="L2" s="3">
         <v>960</v>
@@ -1494,7 +1497,7 @@
         <v>34</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>11</v>
@@ -1511,10 +1514,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E3" s="3">
         <v>11</v>
@@ -1525,13 +1528,13 @@
         <v>1</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L3" s="3">
         <v>780</v>
@@ -1543,7 +1546,7 @@
         <v>39</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>13</v>
@@ -1555,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1566,10 +1569,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E4" s="3">
         <v>13</v>
@@ -1578,13 +1581,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="L4" s="3">
         <v>780</v>
@@ -1596,7 +1599,7 @@
         <v>41</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>16</v>
@@ -1605,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1616,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3">
         <v>15</v>
@@ -1628,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="L5" s="3">
         <v>960</v>
@@ -1643,7 +1646,7 @@
         <v>44</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>17</v>
@@ -1660,10 +1663,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3">
         <v>21</v>
@@ -1672,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L6" s="3">
         <v>780</v>
@@ -1696,7 +1699,7 @@
         <v>12</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1707,28 +1710,28 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E7" s="3">
         <v>24</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L7" s="3">
         <v>780</v>
@@ -1743,7 +1746,7 @@
         <v>20</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>21</v>
@@ -1760,10 +1763,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E8" s="3">
         <v>32</v>
@@ -1774,13 +1777,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L8" s="3">
         <v>780</v>
@@ -1792,7 +1795,7 @@
         <v>108</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>13</v>
@@ -1809,10 +1812,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3">
         <v>39</v>
@@ -1823,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L9" s="3">
         <v>780</v>
@@ -1838,7 +1841,7 @@
         <v>121</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>24</v>
@@ -1858,10 +1861,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E10" s="3">
         <v>41</v>
@@ -1870,10 +1873,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L10" s="3">
         <v>780</v>
@@ -1902,10 +1905,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E11" s="3">
         <v>50</v>
@@ -1916,10 +1919,10 @@
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="L11" s="3">
         <v>780</v>
@@ -1934,13 +1937,13 @@
         <v>29</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1951,10 +1954,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E12" s="3">
         <v>56</v>
@@ -1963,13 +1966,13 @@
         <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="L12" s="3">
         <v>780</v>
@@ -2001,25 +2004,25 @@
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E13" s="3">
         <v>57</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H13" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L13" s="3">
         <v>780</v>
@@ -2031,7 +2034,7 @@
         <v>121</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>34</v>
@@ -2043,7 +2046,7 @@
         <v>26</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -2057,22 +2060,22 @@
         <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E14" s="3">
         <v>63</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L14" s="3">
         <v>780</v>
@@ -2096,7 +2099,7 @@
         <v>39</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -2107,10 +2110,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" s="3">
         <v>73</v>
@@ -2119,31 +2122,28 @@
         <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L15" s="3">
         <v>780</v>
       </c>
       <c r="M15" s="3">
-        <v>900</v>
+        <v>640</v>
       </c>
       <c r="N15" s="3">
         <v>278</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P15" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q15" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -2154,10 +2154,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="E16" s="3">
         <v>78</v>
@@ -2166,7 +2166,13 @@
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>84</v>
+        <v>126</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="L16" s="3">
         <v>780</v>
@@ -2177,20 +2183,12 @@
       <c r="N16" s="7">
         <v>39203</v>
       </c>
-      <c r="O16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="O16" s="3"/>
       <c r="R16" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -2201,10 +2199,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E17" s="3">
         <v>89</v>
@@ -2213,13 +2211,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L17" s="3">
         <v>780</v>
@@ -2251,10 +2249,10 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E18" s="3">
         <v>93</v>
@@ -2263,13 +2261,13 @@
         <v>0</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L18" s="3">
         <v>780</v>
@@ -2281,19 +2279,19 @@
         <v>296</v>
       </c>
       <c r="O18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="R18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="S18" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -2304,10 +2302,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3">
         <v>97</v>
@@ -2316,13 +2314,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L19" s="3">
         <v>780</v>
@@ -2343,7 +2341,7 @@
         <v>28</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
@@ -2351,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -2359,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2447,7 +2445,7 @@
     </row>
     <row r="2" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B2" s="11">
         <v>0</v>
@@ -2506,7 +2504,7 @@
     </row>
     <row r="3" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B3" s="11">
         <v>0</v>
@@ -2565,7 +2563,7 @@
     </row>
     <row r="4" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B4" s="11">
         <v>0</v>
@@ -2624,7 +2622,7 @@
     </row>
     <row r="5" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" s="11">
         <v>0</v>
@@ -2683,7 +2681,7 @@
     </row>
     <row r="6" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B6" s="11">
         <v>0</v>
@@ -2742,7 +2740,7 @@
     </row>
     <row r="7" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="11">
         <v>0</v>
@@ -2801,7 +2799,7 @@
     </row>
     <row r="8" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B8" s="11">
         <v>0</v>
@@ -2860,7 +2858,7 @@
     </row>
     <row r="9" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -2919,7 +2917,7 @@
     </row>
     <row r="10" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B10" s="11">
         <v>0</v>
@@ -2978,7 +2976,7 @@
     </row>
     <row r="11" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B11" s="11">
         <v>0</v>
@@ -3037,7 +3035,7 @@
     </row>
     <row r="12" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B12" s="11">
         <v>0</v>
@@ -3096,7 +3094,7 @@
     </row>
     <row r="13" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -3155,7 +3153,7 @@
     </row>
     <row r="14" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B14" s="11">
         <v>0</v>
@@ -3214,7 +3212,7 @@
     </row>
     <row r="15" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B15" s="11">
         <v>0</v>
@@ -3273,7 +3271,7 @@
     </row>
     <row r="16" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B16" s="11">
         <v>0</v>
@@ -3332,7 +3330,7 @@
     </row>
     <row r="17" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B17" s="11">
         <v>0</v>
@@ -3391,7 +3389,7 @@
     </row>
     <row r="18" spans="1:19" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B18" s="11">
         <v>0</v>

</xml_diff>